<commit_message>
PDF-Status aktualisiert und Pflichtenheft erweitert
</commit_message>
<xml_diff>
--- a/GANTT.xlsx
+++ b/GANTT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\LF9\Projekt 3\LF9_Brandschutz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itellicloud-my.sharepoint.com/personal/max_ullmann_bs_nttdata_com/Documents/Dokumente/Berufsschule/LF9/LF9_Brandschutz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B9CFC6-24C0-4BFE-B7D5-BADBFFDCB300}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B9CFC6-24C0-4BFE-B7D5-BADBFFDCB300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{76A922F1-B1E7-4ABD-8EC0-B8A3949F5B79}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76A922F1-B1E7-4ABD-8EC0-B8A3949F5B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -141,17 +141,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -159,11 +150,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="40 % - Akzent1" xfId="2" builtinId="31"/>
-    <cellStyle name="60 % - Akzent3" xfId="1" builtinId="40"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -477,36 +477,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44955EC7-D8A4-4860-A995-0ED540D2F4C6}">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A16" sqref="A16"/>
+      <selection pane="topRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -523,56 +523,56 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="5" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="7" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="8"/>
+      <c r="Q2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="5" t="s">
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="3" t="s">
+      <c r="W2" s="8"/>
+      <c r="X2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="5" t="s">
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="5"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="AD2" s="8"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -603,8 +603,8 @@
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1">
         <v>44893</v>
@@ -621,10 +621,10 @@
       <c r="G4" s="1">
         <v>44897</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>44898</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>44899</v>
       </c>
       <c r="J4" s="1">
@@ -642,10 +642,10 @@
       <c r="N4" s="1">
         <v>44904</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="4">
         <v>44905</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="4">
         <v>44576</v>
       </c>
       <c r="Q4" s="1">
@@ -663,10 +663,10 @@
       <c r="U4" s="1">
         <v>44581</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="4">
         <v>44582</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="4">
         <v>44583</v>
       </c>
       <c r="X4" s="1">
@@ -684,19 +684,19 @@
       <c r="AB4" s="1">
         <v>44588</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AC4" s="4">
         <v>44589</v>
       </c>
       <c r="AD4" s="2"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="O5" s="2"/>
@@ -706,14 +706,14 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="O6" s="2"/>
@@ -723,14 +723,14 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="4"/>
+      <c r="J7" s="3"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="V7" s="2"/>
@@ -738,14 +738,14 @@
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="K8" s="4"/>
+      <c r="K8" s="3"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="V8" s="2"/>
@@ -753,15 +753,15 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="V9" s="2"/>
@@ -769,15 +769,15 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="V10" s="2"/>
@@ -785,8 +785,8 @@
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2"/>
@@ -794,15 +794,15 @@
       <c r="I11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
     </row>
-    <row r="12" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="2"/>
@@ -810,15 +810,15 @@
       <c r="I12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2"/>
@@ -826,15 +826,15 @@
       <c r="I13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
     </row>
-    <row r="14" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2"/>
@@ -844,13 +844,13 @@
       <c r="P14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
     </row>
-    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2"/>
@@ -860,41 +860,41 @@
       <c r="P15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
     </row>
-    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:N2"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>